<commit_message>
Created first successful validated EML file for EDI publication
</commit_message>
<xml_diff>
--- a/Data paper/Biomass conversions.xlsx
+++ b/Data paper/Biomass conversions.xlsx
@@ -8,25 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\ZoopSynth\Data paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745394A4-3B73-4F1E-A60D-7F13B8B06962}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70BA44F-FCEA-4926-9200-3020138AB3F3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15264" yWindow="-2604" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15264" yWindow="-2604" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Micro and Meso-zooplankton" sheetId="2" r:id="rId1"/>
     <sheet name="Macro-zooplankton" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="58">
   <si>
     <t>Taxname</t>
   </si>
@@ -40,9 +46,6 @@
     <t>CarbonWeight_ug</t>
   </si>
   <si>
-    <t>Source</t>
-  </si>
-  <si>
     <t>Limnoithona</t>
   </si>
   <si>
@@ -124,9 +127,6 @@
     <t>Oithona</t>
   </si>
   <si>
-    <t>Uye S, Sano K. 1995. Seasonal reproductive biology of the small cyclopoid copepod Oithona. Mar Ecol Prog Ser. 118(Uchima 198513):121–128.</t>
-  </si>
-  <si>
     <t>Oithona davisae</t>
   </si>
   <si>
@@ -139,9 +139,6 @@
     <t>Pseudodiaptomus</t>
   </si>
   <si>
-    <t>Growth and production of the inshore marine copepod Pseudodiaptomus marinus in the central part of the Inland Sea of Japan</t>
-  </si>
-  <si>
     <t>Pseudodiaptomus forbesi</t>
   </si>
   <si>
@@ -194,6 +191,21 @@
   </si>
   <si>
     <t>Kimmerer et al. 2011 Length, weight, carbon, and nitrogen content of common copepods in the San Francisco Estuary</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Kimmerer, W. J., T. R. Ignoffo, K. R. Kayfetz, and A. M. Slaughter. 2018. Effects of freshwater flow and phytoplankton biomass on growth, reproduction, and spatial subsidies of the estuarine copepod Pseudodiaptomus forbesi. Hydrobiologia 807:113–130.</t>
+  </si>
+  <si>
+    <t>Gould, A. L., and W. J. Kimmerer. 2010. Development, growth, and reproduction of the cyclopoid copepod Limnoithona tetraspina in the upper San Francisco Estuary. Marine Ecology Progress Series 412:163–177.</t>
+  </si>
+  <si>
+    <t>Uye, S., and K. Sano. 1995. Seasonal reproductive biology of the small cyclopoid copepod Oithona davisae in a temperate eutrophic inlet. Marine Ecology Progress Series 118:121–128.</t>
+  </si>
+  <si>
+    <t>Uye, S., Y. Iwai, and S. Kasahara. 1983. Growth and production of the inshore marine copepod Pseudodiaptomus marinus in the central part of the Inland Sea of Japan. Marine Biology 73:91–98.</t>
   </si>
 </sst>
 </file>
@@ -307,7 +319,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
@@ -338,6 +350,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -622,11 +635,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13C544B-28E0-4ED3-8459-C8F5B3BB063B}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,466 +664,483 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="D2" s="4">
         <v>0.04</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="D3" s="6">
         <v>1.3009999999999999</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="6">
         <v>2.984</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="7">
         <v>1.1619999999999999</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="6">
         <v>2.6659999999999999</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="7">
         <v>0.6</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="D8" s="7">
         <v>3.8</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="7">
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="7">
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" s="7">
         <v>1.4430000000000001</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" s="7">
         <v>3.55</v>
       </c>
       <c r="E13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D14" s="7">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="C15" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D15" s="7">
         <v>0.13300000000000001</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16" s="7">
         <v>0.13300000000000001</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" s="7">
-        <v>0.13300000000000001</v>
+        <v>8.8663036902600939E-2</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="D18" s="7">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="E18" t="s">
-        <v>32</v>
+        <v>4.5952813067150579E-2</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="D19" s="7">
-        <v>0.20100000000000001</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>55</v>
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20" s="7">
-        <v>0.23</v>
-      </c>
-      <c r="E20" t="s">
-        <v>34</v>
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="9">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>34</v>
+        <v>8</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0.23</v>
+      </c>
+      <c r="E21" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>37</v>
+        <v>8</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D23" s="7">
-        <v>1.252</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>55</v>
+        <v>0.1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D24" s="7">
-        <v>2.6619999999999999</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>55</v>
+        <v>1.24</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D25" s="7">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="E25" t="s">
-        <v>37</v>
+        <v>3.2650000000000001</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D26" s="7">
-        <v>1.8109999999999999</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>55</v>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E26" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D27" s="7">
-        <v>3.4129999999999998</v>
+        <v>1.8109999999999999</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D28" s="7">
+        <v>3.4129999999999998</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="7">
         <v>18.690000000000001</v>
       </c>
-      <c r="E28" s="11" t="s">
-        <v>42</v>
+      <c r="E29" s="11" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1122,8 +1152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E689D54-14E1-4511-9AF6-F8307BF390D6}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,24 +1176,24 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>9.9599999999999995E-6</v>
@@ -1172,18 +1202,18 @@
         <v>3.1283667400000001</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>2.0829999999999999E-5</v>
@@ -1192,18 +1222,18 @@
         <v>2.8084990300000001</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>2.2969999999999999E-5</v>
@@ -1212,18 +1242,18 @@
         <v>2.7306027899999998</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <v>2.546E-5</v>
@@ -1232,18 +1262,18 @@
         <v>2.6659406099999998</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>1.1999999999999999E-3</v>
@@ -1252,18 +1282,18 @@
         <v>3.2532999999999999</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>4.5199999999999999E-6</v>
@@ -1272,18 +1302,18 @@
         <v>3.3163180300000001</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>2.2039999999999999E-5</v>
@@ -1292,18 +1322,18 @@
         <v>2.8256118799999999</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <v>2.3900000000000002E-5</v>
@@ -1312,18 +1342,18 @@
         <v>2.7388844300000001</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <v>2.7180000000000001E-5</v>
@@ -1332,7 +1362,7 @@
         <v>2.6669142099999998</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on updating biomass table
</commit_message>
<xml_diff>
--- a/Data paper/Biomass conversions.xlsx
+++ b/Data paper/Biomass conversions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\ZoopSynth\Data paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46349C3A-A008-449E-A7DE-2F06BBBF335D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3843CA11-E9D2-468D-9796-F30B8C37C86F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Micro and Meso-zooplankton" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="69">
   <si>
     <t>Taxname</t>
   </si>
@@ -212,6 +212,33 @@
   </si>
   <si>
     <t>b_dry</t>
+  </si>
+  <si>
+    <t>CDFW mysid matrix</t>
+  </si>
+  <si>
+    <t>Chigbu and Sibley 1996</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Formalin</t>
+  </si>
+  <si>
+    <t>Ethanol</t>
+  </si>
+  <si>
+    <t>Preservative_wet</t>
+  </si>
+  <si>
+    <t>Preservative_dry</t>
+  </si>
+  <si>
+    <t>Reference_wet</t>
+  </si>
+  <si>
+    <t>Reference_dry</t>
   </si>
 </sst>
 </file>
@@ -325,7 +352,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
@@ -357,6 +384,11 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -643,9 +675,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13C544B-28E0-4ED3-8459-C8F5B3BB063B}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,23 +1188,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E689D54-14E1-4511-9AF6-F8307BF390D6}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
+    <col min="10" max="10" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1195,10 +1231,19 @@
         <v>59</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>40</v>
       </c>
@@ -1214,173 +1259,366 @@
       <c r="E2">
         <v>3.1283667400000001</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" s="13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>1.844E-5</v>
+      </c>
+      <c r="E3">
+        <v>3.0299096799999998</v>
+      </c>
+      <c r="H3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3">
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
         <v>2.0829999999999999E-5</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>2.8084990300000001</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>3.1109999999999999E-5</v>
+      </c>
+      <c r="E5">
+        <v>2.63742762</v>
+      </c>
+      <c r="H5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4">
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
         <v>2.2969999999999999E-5</v>
       </c>
-      <c r="E4">
+      <c r="E6">
         <v>2.7306027899999998</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>2.0800000000000001E-5</v>
+      </c>
+      <c r="E7">
+        <v>2.9264617799999999</v>
+      </c>
+      <c r="H7" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5">
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8">
         <v>2.546E-5</v>
       </c>
-      <c r="E5">
+      <c r="E8">
         <v>2.6659406099999998</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>1.3699999999999999E-5</v>
+      </c>
+      <c r="E9">
+        <v>3.1582650399999999</v>
+      </c>
+      <c r="H9" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6">
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <f>EXP(-6.08)</f>
+        <v>2.2881766529221693E-3</v>
+      </c>
+      <c r="E10">
+        <v>3.45</v>
+      </c>
+      <c r="F10">
+        <f>EXP(-5.02)</f>
+        <v>6.6045267093148112E-3</v>
+      </c>
+      <c r="G10">
+        <v>2.57</v>
+      </c>
+      <c r="H10" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" t="s">
+        <v>62</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="E6">
+      <c r="G11">
         <v>3.2532999999999999</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="J11" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>4.5199999999999999E-6</v>
+      </c>
+      <c r="E12">
+        <v>3.3163180300000001</v>
+      </c>
+      <c r="F12">
+        <v>1.03E-2</v>
+      </c>
+      <c r="G12">
+        <v>2.2593000000000001</v>
+      </c>
+      <c r="H12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="13" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>4.5199999999999999E-6</v>
-      </c>
-      <c r="E7">
-        <v>3.3163180300000001</v>
-      </c>
-      <c r="F7">
-        <v>1.03E-2</v>
-      </c>
-      <c r="G7">
-        <v>2.2593000000000001</v>
-      </c>
-      <c r="H7" s="13" t="s">
+      <c r="K12" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>2.2039999999999999E-5</v>
+      </c>
+      <c r="E13">
+        <v>2.8256118799999999</v>
+      </c>
+      <c r="H13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <v>2.2039999999999999E-5</v>
-      </c>
-      <c r="E8">
-        <v>2.8256118799999999</v>
-      </c>
-      <c r="H8" s="13" t="s">
+      <c r="B14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>3.79E-5</v>
+      </c>
+      <c r="E14">
+        <v>2.55030073</v>
+      </c>
+      <c r="H14" t="s">
+        <v>64</v>
+      </c>
+      <c r="J14" s="13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9">
+      <c r="B15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15">
         <v>2.3900000000000002E-5</v>
       </c>
-      <c r="E9">
+      <c r="E15">
         <v>2.7388844300000001</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H15" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10">
+      <c r="B16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17">
         <v>2.7180000000000001E-5</v>
       </c>
-      <c r="E10">
+      <c r="E17">
         <v>2.6669142099999998</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H17" t="s">
+        <v>64</v>
+      </c>
+      <c r="J17" s="13" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating readme and biomass table
</commit_message>
<xml_diff>
--- a/Data paper/Biomass conversions.xlsx
+++ b/Data paper/Biomass conversions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\ZoopSynth\Data paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9699EF-7E7B-4729-BC79-29BC1E35E03C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD7869A-F40B-4E46-A32C-2A0A29F5498D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3780" yWindow="8865" windowWidth="53445" windowHeight="22380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-240" yWindow="-240" windowWidth="38880" windowHeight="21480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Micro and Meso-zooplankton" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="74">
   <si>
     <t>Taxname</t>
   </si>
@@ -697,18 +697,18 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
+      <selection pane="bottomLeft" sqref="A1:E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="213" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -725,7 +725,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -742,7 +742,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -759,7 +759,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -776,7 +776,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -793,7 +793,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -810,7 +810,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -827,7 +827,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -844,7 +844,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -861,7 +861,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -878,7 +878,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -895,7 +895,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
@@ -912,7 +912,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -929,7 +929,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -946,7 +946,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
@@ -963,7 +963,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
@@ -980,7 +980,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
@@ -997,7 +997,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>31</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>33</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>34</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>35</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>37</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>37</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>38</v>
       </c>
@@ -1208,798 +1208,802 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E689D54-14E1-4511-9AF6-F8307BF390D6}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="J24" sqref="A1:J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.3125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1015625" customWidth="1"/>
-    <col min="5" max="5" width="11.3671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="10.20703125" customWidth="1"/>
-    <col min="8" max="8" width="10.47265625" customWidth="1"/>
-    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.68359375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.15625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="18" t="s">
+      <c r="C1" s="18" t="s">
         <v>69</v>
       </c>
+      <c r="D1" s="17" t="s">
+        <v>59</v>
+      </c>
       <c r="E1" s="17" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" s="17" t="s">
         <v>67</v>
       </c>
+      <c r="H1" s="18" t="s">
+        <v>62</v>
+      </c>
       <c r="I1" s="18" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="K1" s="18" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="19" t="s">
+      <c r="C2" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="D2" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="13">
+      <c r="E2" s="3">
         <v>200</v>
       </c>
-      <c r="G2" s="13">
+      <c r="F2" s="3">
         <v>2</v>
       </c>
-      <c r="H2" s="13">
+      <c r="G2" s="3">
         <v>9</v>
       </c>
+      <c r="H2" s="19">
+        <v>1.03E-2</v>
+      </c>
       <c r="I2" s="19">
-        <v>1.03E-2</v>
-      </c>
-      <c r="J2" s="19">
         <v>2.2593000000000001</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="J2" s="20" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>44</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="19" t="s">
+      <c r="C3" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="13">
+      <c r="E3" s="3">
         <v>700</v>
       </c>
-      <c r="G3" s="13">
+      <c r="F3" s="3">
         <v>2</v>
       </c>
-      <c r="H3" s="13">
+      <c r="G3" s="3">
         <v>16</v>
       </c>
+      <c r="H3" s="19">
+        <v>1.1999999999999999E-3</v>
+      </c>
       <c r="I3" s="19">
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="J3" s="19">
         <v>3.2532999999999999</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="J3" s="20" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>44</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="19" t="s">
+      <c r="C4" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="D4" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="13">
+      <c r="E4" s="3">
         <v>63</v>
       </c>
-      <c r="G4" s="13">
+      <c r="F4" s="3">
         <v>7.4</v>
       </c>
-      <c r="H4" s="13">
+      <c r="G4" s="3">
         <v>16.399999999999999</v>
       </c>
-      <c r="I4" s="19">
+      <c r="H4" s="19">
         <f>EXP(-5.02)</f>
         <v>6.6045267093148112E-3</v>
       </c>
-      <c r="J4" s="19">
+      <c r="I4" s="19">
         <v>2.57</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="J4" s="21" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>46</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="19" t="s">
+      <c r="C5" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="D5" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="20">
+      <c r="E5" s="20">
         <v>108</v>
       </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
+      <c r="F5" s="3">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="H5" s="19">
+        <v>3.2979999999999999E-5</v>
+      </c>
       <c r="I5" s="19">
-        <v>3.2979999999999999E-5</v>
-      </c>
-      <c r="J5" s="19">
         <v>2.64586524</v>
       </c>
-      <c r="K5" s="20" t="s">
+      <c r="J5" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>48</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="19" t="s">
+      <c r="C6" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="D6" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="20">
+      <c r="E6" s="20">
         <v>25</v>
       </c>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
+      <c r="F6" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="H6" s="19">
+        <v>3.1690000000000003E-5</v>
+      </c>
       <c r="I6" s="19">
-        <v>3.1690000000000003E-5</v>
-      </c>
-      <c r="J6" s="19">
         <v>2.4761398300000002</v>
       </c>
-      <c r="K6" s="20" t="s">
+      <c r="J6" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="19" t="s">
+      <c r="C7" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="D7" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="20">
+      <c r="E7" s="20">
         <v>361</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
+      <c r="F7" s="3">
+        <v>1.9</v>
+      </c>
+      <c r="G7" s="3">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="H7" s="19">
+        <v>2.0769999999999999E-5</v>
+      </c>
       <c r="I7" s="19">
-        <v>2.0769999999999999E-5</v>
-      </c>
-      <c r="J7" s="19">
         <v>2.9079799999999998</v>
       </c>
-      <c r="K7" s="20" t="s">
+      <c r="J7" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>41</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="19" t="s">
+      <c r="C8" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="D8" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="20">
+      <c r="E8" s="20">
         <v>155</v>
       </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
+      <c r="F8" s="3">
+        <v>2</v>
+      </c>
+      <c r="G8" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="H8" s="19">
+        <v>3.1550000000000001E-5</v>
+      </c>
       <c r="I8" s="19">
-        <v>3.1550000000000001E-5</v>
-      </c>
-      <c r="J8" s="19">
         <v>2.6111537999999999</v>
       </c>
-      <c r="K8" s="20" t="s">
+      <c r="J8" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>71</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="19" t="s">
+      <c r="C9" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="D9" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="20">
+      <c r="E9" s="20">
         <v>37</v>
       </c>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
+      <c r="F9" s="19">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G9" s="19">
+        <v>5.5</v>
+      </c>
+      <c r="H9" s="19">
+        <v>9.2599999999999994E-6</v>
+      </c>
       <c r="I9" s="19">
-        <v>9.2599999999999994E-6</v>
-      </c>
-      <c r="J9" s="19">
         <v>3.2843297300000001</v>
       </c>
-      <c r="K9" s="20" t="s">
+      <c r="J9" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="19" t="s">
+      <c r="C10" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="D10" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="20">
+      <c r="E10" s="20">
         <v>207</v>
       </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
+      <c r="F10" s="3">
+        <v>1.9</v>
+      </c>
+      <c r="G10" s="3">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="H10" s="19">
+        <v>1.5659999999999999E-5</v>
+      </c>
       <c r="I10" s="19">
-        <v>1.5659999999999999E-5</v>
-      </c>
-      <c r="J10" s="19">
         <v>3.0731050099999999</v>
       </c>
-      <c r="K10" s="20" t="s">
+      <c r="J10" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="19" t="s">
+      <c r="C11" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="D11" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="20">
+      <c r="E11" s="20">
         <v>84</v>
       </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
+      <c r="F11" s="3">
+        <v>2</v>
+      </c>
+      <c r="G11" s="3">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="H11" s="19">
+        <v>1.2469999999999999E-5</v>
+      </c>
       <c r="I11" s="19">
-        <v>1.2469999999999999E-5</v>
-      </c>
-      <c r="J11" s="19">
         <v>3.2246936100000001</v>
       </c>
-      <c r="K11" s="20" t="s">
+      <c r="J11" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>72</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="19" t="s">
+      <c r="C12" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="D12" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="20">
+      <c r="E12" s="20">
         <v>39</v>
       </c>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
+      <c r="F12" s="19">
+        <v>1.9</v>
+      </c>
+      <c r="G12" s="19">
+        <v>10</v>
+      </c>
+      <c r="H12" s="19">
+        <v>3.3429999999999997E-5</v>
+      </c>
       <c r="I12" s="19">
-        <v>3.3429999999999997E-5</v>
-      </c>
-      <c r="J12" s="19">
         <v>2.5935991700000001</v>
       </c>
-      <c r="K12" s="20" t="s">
+      <c r="J12" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="19" t="s">
+      <c r="C13" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="D13" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="13">
+      <c r="E13" s="3">
         <v>50</v>
       </c>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
+      <c r="F13" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="G13" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="H13" s="19">
+        <v>2.8690000000000001E-5</v>
+      </c>
       <c r="I13" s="19">
-        <v>2.8690000000000001E-5</v>
-      </c>
-      <c r="J13" s="19">
         <v>2.5994960699999998</v>
       </c>
-      <c r="K13" s="20" t="s">
+      <c r="J13" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>73</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="19" t="s">
+      <c r="C14" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="D14" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="20">
+      <c r="E14" s="20">
         <v>19</v>
       </c>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
+      <c r="F14" s="19">
+        <v>2</v>
+      </c>
+      <c r="G14" s="19">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H14" s="19">
+        <v>2.5049999999999999E-5</v>
+      </c>
       <c r="I14" s="19">
-        <v>2.5049999999999999E-5</v>
-      </c>
-      <c r="J14" s="19">
         <v>2.6410646799999999</v>
       </c>
-      <c r="K14" s="20" t="s">
+      <c r="J14" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="19" t="s">
+      <c r="C15" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="D15" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="22">
-        <v>113</v>
-      </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
+      <c r="E15" s="22">
+        <v>114</v>
+      </c>
+      <c r="F15" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G15" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="H15" s="19">
+        <v>2.2039999999999999E-5</v>
+      </c>
       <c r="I15" s="19">
-        <v>2.2039999999999999E-5</v>
-      </c>
-      <c r="J15" s="19">
         <v>2.8256118799999999</v>
       </c>
-      <c r="K15" s="20" t="s">
+      <c r="J15" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="19" t="s">
+      <c r="C16" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="D16" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F16" s="22">
+      <c r="E16" s="22">
         <v>52</v>
       </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
+      <c r="F16" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>5.3</v>
+      </c>
+      <c r="H16" s="19">
+        <v>5.7510000000000003E-5</v>
+      </c>
       <c r="I16" s="19">
-        <v>5.7510000000000003E-5</v>
-      </c>
-      <c r="J16" s="19">
         <v>1.9935650600000001</v>
       </c>
-      <c r="K16" s="20" t="s">
+      <c r="J16" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>47</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="19" t="s">
+      <c r="C17" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="D17" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="22">
+      <c r="E17" s="22">
         <v>196</v>
       </c>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
+      <c r="F17" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="G17" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="H17" s="19">
+        <v>2.3900000000000002E-5</v>
+      </c>
       <c r="I17" s="19">
-        <v>2.3900000000000002E-5</v>
-      </c>
-      <c r="J17" s="19">
         <v>2.7388844300000001</v>
       </c>
-      <c r="K17" s="20" t="s">
+      <c r="J17" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="19" t="s">
+      <c r="C18" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="D18" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="22">
+      <c r="E18" s="22">
         <v>597</v>
       </c>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
+      <c r="F18" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="G18" s="3">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="H18" s="19">
+        <v>2.2969999999999999E-5</v>
+      </c>
       <c r="I18" s="19">
-        <v>2.2969999999999999E-5</v>
-      </c>
-      <c r="J18" s="19">
         <v>2.7306027899999998</v>
       </c>
-      <c r="K18" s="20" t="s">
+      <c r="J18" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>41</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="19" t="s">
+      <c r="C19" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="D19" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F19" s="22">
+      <c r="E19" s="22">
         <v>290</v>
       </c>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
+      <c r="F19" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="G19" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="H19" s="19">
+        <v>2.0829999999999999E-5</v>
+      </c>
       <c r="I19" s="19">
-        <v>2.0829999999999999E-5</v>
-      </c>
-      <c r="J19" s="19">
         <v>2.8084990300000001</v>
       </c>
-      <c r="K19" s="20" t="s">
+      <c r="J19" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="19" t="s">
+      <c r="C20" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="D20" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="22">
+      <c r="E20" s="22">
         <v>306</v>
       </c>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
+      <c r="F20" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="G20" s="3">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="H20" s="19">
+        <v>2.546E-5</v>
+      </c>
       <c r="I20" s="19">
-        <v>2.546E-5</v>
-      </c>
-      <c r="J20" s="19">
         <v>2.6659406099999998</v>
       </c>
-      <c r="K20" s="20" t="s">
+      <c r="J20" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="19" t="s">
+      <c r="C21" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="D21" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F21" s="22">
+      <c r="E21" s="22">
         <v>105</v>
       </c>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
+      <c r="F21" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="G21" s="3">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="H21" s="19">
+        <v>9.9599999999999995E-6</v>
+      </c>
       <c r="I21" s="19">
-        <v>9.9599999999999995E-6</v>
-      </c>
-      <c r="J21" s="19">
         <v>3.1283667400000001</v>
       </c>
-      <c r="K21" s="20" t="s">
+      <c r="J21" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="19" t="s">
+      <c r="C22" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="D22" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F22" s="13">
-        <v>108</v>
-      </c>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
+      <c r="E22" s="3">
+        <v>100</v>
+      </c>
+      <c r="F22" s="3">
+        <v>2.9</v>
+      </c>
+      <c r="G22" s="3">
+        <v>11</v>
+      </c>
+      <c r="H22" s="19">
+        <v>3.4999999999999999E-6</v>
+      </c>
       <c r="I22" s="19">
-        <v>3.4999999999999999E-6</v>
-      </c>
-      <c r="J22" s="19">
         <v>3.4633203899999998</v>
       </c>
-      <c r="K22" s="20" t="s">
+      <c r="J22" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>70</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="19" t="s">
+      <c r="C23" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="D23" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F23" s="22">
-        <v>108</v>
-      </c>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
+      <c r="E23" s="22">
+        <v>107</v>
+      </c>
+      <c r="F23" s="19">
+        <v>2.1</v>
+      </c>
+      <c r="G23" s="19">
+        <v>3.9</v>
+      </c>
+      <c r="H23" s="19">
+        <v>1.9259999999999999E-5</v>
+      </c>
       <c r="I23" s="19">
-        <v>1.9259999999999999E-5</v>
-      </c>
-      <c r="J23" s="19">
         <v>2.7779618099999999</v>
       </c>
-      <c r="K23" s="20" t="s">
+      <c r="J23" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>44</v>
       </c>
       <c r="B24" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="19" t="s">
+      <c r="C24" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="D24" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F24" s="13">
+      <c r="E24" s="3">
         <v>63</v>
       </c>
-      <c r="G24" s="13">
+      <c r="F24" s="3">
         <v>7.4</v>
       </c>
-      <c r="H24" s="13">
+      <c r="G24" s="3">
         <v>16.399999999999999</v>
       </c>
-      <c r="I24" s="19">
+      <c r="H24" s="19">
         <f>EXP(-6.08)</f>
         <v>2.2881766529221693E-3</v>
       </c>
-      <c r="J24" s="19">
+      <c r="I24" s="19">
         <v>3.45</v>
       </c>
-      <c r="K24" s="21" t="s">
+      <c r="J24" s="21" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K24">
-    <sortCondition ref="E2:E24"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J24">
     <sortCondition ref="D2:D24"/>
+    <sortCondition ref="C2:C24"/>
     <sortCondition ref="A2:A24"/>
-    <sortCondition ref="K2:K24"/>
+    <sortCondition ref="J2:J24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed error in biomass conversions
</commit_message>
<xml_diff>
--- a/Data paper/Biomass conversions.xlsx
+++ b/Data paper/Biomass conversions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\ZoopSynth\Data paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD7869A-F40B-4E46-A32C-2A0A29F5498D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98E5BCB-3416-4497-BE59-E232E7BB52D2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-240" yWindow="-240" windowWidth="38880" windowHeight="21480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4005" windowWidth="36030" windowHeight="16995" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Micro and Meso-zooplankton" sheetId="2" r:id="rId1"/>
@@ -163,9 +163,6 @@
     <t>Amphipoda</t>
   </si>
   <si>
-    <t>Gammarus</t>
-  </si>
-  <si>
     <t>Neomysis mercedis</t>
   </si>
   <si>
@@ -254,6 +251,9 @@
   </si>
   <si>
     <t>Sinocorophium alienense</t>
+  </si>
+  <si>
+    <t>Gammaridae</t>
   </si>
 </sst>
 </file>
@@ -722,7 +722,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -739,7 +739,7 @@
         <v>0.04</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -756,7 +756,7 @@
         <v>1.3009999999999999</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -773,7 +773,7 @@
         <v>2.984</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -790,7 +790,7 @@
         <v>1.1619999999999999</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -807,7 +807,7 @@
         <v>2.6659999999999999</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -909,7 +909,7 @@
         <v>1.4430000000000001</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -960,7 +960,7 @@
         <v>0.13300000000000001</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -977,7 +977,7 @@
         <v>0.13300000000000001</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -994,7 +994,7 @@
         <v>8.8663036902600939E-2</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1011,7 +1011,7 @@
         <v>4.5952813067150579E-2</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1028,7 +1028,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="E19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1045,7 +1045,7 @@
         <v>0.20100000000000001</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1096,7 +1096,7 @@
         <v>0.1</v>
       </c>
       <c r="E23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1113,7 +1113,7 @@
         <v>1.24</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1130,7 +1130,7 @@
         <v>3.2650000000000001</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1147,7 +1147,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="E26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1164,7 +1164,7 @@
         <v>1.8109999999999999</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1181,7 +1181,7 @@
         <v>3.4129999999999998</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1211,12 +1211,12 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="A1:J24"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.140625" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" customWidth="1"/>
@@ -1236,42 +1236,42 @@
         <v>1</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="17" t="s">
-        <v>67</v>
-      </c>
       <c r="H1" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="18" t="s">
-        <v>63</v>
-      </c>
       <c r="J1" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" s="3">
         <v>200</v>
@@ -1289,21 +1289,21 @@
         <v>2.2593000000000001</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="3">
         <v>700</v>
@@ -1321,21 +1321,21 @@
         <v>3.2532999999999999</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" s="3">
         <v>63</v>
@@ -1354,21 +1354,21 @@
         <v>2.57</v>
       </c>
       <c r="J4" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" s="20">
         <v>108</v>
@@ -1386,21 +1386,21 @@
         <v>2.64586524</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" s="20">
         <v>25</v>
@@ -1418,7 +1418,7 @@
         <v>2.4761398300000002</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1429,10 +1429,10 @@
         <v>26</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E7" s="20">
         <v>361</v>
@@ -1450,7 +1450,7 @@
         <v>2.9079799999999998</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1461,10 +1461,10 @@
         <v>21</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E8" s="20">
         <v>155</v>
@@ -1482,21 +1482,21 @@
         <v>2.6111537999999999</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E9" s="20">
         <v>37</v>
@@ -1514,21 +1514,21 @@
         <v>3.2843297300000001</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" s="20">
         <v>207</v>
@@ -1546,7 +1546,7 @@
         <v>3.0731050099999999</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="20">
         <v>84</v>
@@ -1578,21 +1578,21 @@
         <v>3.2246936100000001</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" s="20">
         <v>39</v>
@@ -1610,21 +1610,21 @@
         <v>2.5935991700000001</v>
       </c>
       <c r="J12" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E13" s="3">
         <v>50</v>
@@ -1642,21 +1642,21 @@
         <v>2.5994960699999998</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E14" s="20">
         <v>19</v>
@@ -1674,21 +1674,21 @@
         <v>2.6410646799999999</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E15" s="22">
         <v>114</v>
@@ -1706,21 +1706,21 @@
         <v>2.8256118799999999</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E16" s="22">
         <v>52</v>
@@ -1738,21 +1738,21 @@
         <v>1.9935650600000001</v>
       </c>
       <c r="J16" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E17" s="22">
         <v>196</v>
@@ -1770,7 +1770,7 @@
         <v>2.7388844300000001</v>
       </c>
       <c r="J17" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1781,10 +1781,10 @@
         <v>26</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E18" s="22">
         <v>597</v>
@@ -1802,7 +1802,7 @@
         <v>2.7306027899999998</v>
       </c>
       <c r="J18" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1813,10 +1813,10 @@
         <v>21</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19" s="22">
         <v>290</v>
@@ -1834,21 +1834,21 @@
         <v>2.8084990300000001</v>
       </c>
       <c r="J19" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E20" s="22">
         <v>306</v>
@@ -1866,7 +1866,7 @@
         <v>2.6659406099999998</v>
       </c>
       <c r="J20" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1877,10 +1877,10 @@
         <v>10</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E21" s="22">
         <v>105</v>
@@ -1898,21 +1898,21 @@
         <v>3.1283667400000001</v>
       </c>
       <c r="J21" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E22" s="3">
         <v>100</v>
@@ -1930,21 +1930,21 @@
         <v>3.4633203899999998</v>
       </c>
       <c r="J22" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E23" s="22">
         <v>107</v>
@@ -1962,21 +1962,21 @@
         <v>2.7779618099999999</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E24" s="3">
         <v>63</v>
@@ -1995,7 +1995,7 @@
         <v>3.45</v>
       </c>
       <c r="J24" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>